<commit_message>
updated some more analysis part
</commit_message>
<xml_diff>
--- a/cod.xlsx
+++ b/cod.xlsx
@@ -2242,9 +2242,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1389960</xdr:colOff>
+      <xdr:colOff>1389600</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>177120</xdr:rowOff>
+      <xdr:rowOff>176760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2258,7 +2258,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="57240" y="50760"/>
-          <a:ext cx="1332720" cy="326160"/>
+          <a:ext cx="1332360" cy="325800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2454,22 +2454,27 @@
   </sheetPr>
   <dimension ref="A1:BA389"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A154" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B144" activeCellId="0" sqref="B144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1339285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1428571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.6875"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.4642857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.4642857142857"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.3392857142857"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.75"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="53" min="19" style="0" width="12.9910714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.8928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7901785714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.56696428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.15625"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3482142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.3482142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.2232142857143"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.6294642857143"/>
+    <col collapsed="false" hidden="false" max="15" min="12" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.15625"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="53" min="19" style="0" width="12.7589285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="54" style="0" width="8.50446428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -65128,19 +65133,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.78125"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.15625"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="11.5758928571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6919642857143"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="11.2232142857143"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.56696428571429"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.6294642857143"/>
-    <col collapsed="false" hidden="false" max="33" min="18" style="0" width="10.9866071428571"/>
-    <col collapsed="false" hidden="false" max="36" min="35" style="0" width="11.4553571428571"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="10.15625"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="11.9285714285714"/>
-    <col collapsed="false" hidden="false" max="46" min="45" style="0" width="11.1026785714286"/>
-    <col collapsed="false" hidden="false" max="50" min="49" style="0" width="11.2232142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.3080357142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.92410714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="11.4553571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5758928571429"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="11.1026785714286"/>
+    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.45089285714286"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="33" min="18" style="0" width="10.8660714285714"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="36" min="35" style="0" width="11.3392857142857"/>
+    <col collapsed="false" hidden="false" max="40" min="37" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="9.92410714285714"/>
+    <col collapsed="false" hidden="false" max="43" min="42" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="11.6919642857143"/>
+    <col collapsed="false" hidden="false" max="46" min="45" style="0" width="10.9866071428571"/>
+    <col collapsed="false" hidden="false" max="48" min="47" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="50" min="49" style="0" width="11.1026785714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="51" style="0" width="8.50446428571429"/>
   </cols>
   <sheetData>
     <row r="1" s="22" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>